<commit_message>
redesigned the spell checking class. It was causing a memory shortage. Now it functions way more efficently.
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -569,6 +569,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42587.832430555558</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created a thread safe log textbox
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -897,6 +897,293 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42601.977083333331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42601.988379629627</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42601.988946759258</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42601.99114583333</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42601.995023148149</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>66</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>100</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42601.997997685183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42601.999166666668</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I changed the name of the word files. This will make it easier to edit them. I also changed the message that is printed to the text box
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1471,6 +1471,129 @@
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42602.513611111113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>100</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42602.516736111109</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>18</v>
+      </c>
+      <c r="D28">
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>100</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>100</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42602.524085648147</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>63</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>100</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>100</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more to the word lists. removed innovate as it ca be a false poritive. Changed the test articles
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/EXAMPLEEXCEL1/EXAMPLEEXCEL1Bag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1594,6 +1594,129 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42602.576064814813</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>163</v>
+      </c>
+      <c r="D30">
+        <v>338</v>
+      </c>
+      <c r="E30">
+        <v>31</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>16</v>
+      </c>
+      <c r="H30">
+        <v>30</v>
+      </c>
+      <c r="I30">
+        <v>69</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42602.576898148145</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>144</v>
+      </c>
+      <c r="D31">
+        <v>338</v>
+      </c>
+      <c r="E31">
+        <v>31</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>16</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+      <c r="I31">
+        <v>69</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42602.577210648145</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>138</v>
+      </c>
+      <c r="D32">
+        <v>338</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>18</v>
+      </c>
+      <c r="H32">
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <v>81</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>